<commit_message>
Added feature to copy lists and move to different board
</commit_message>
<xml_diff>
--- a/Java Requirements.xlsx
+++ b/Java Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00495F73-6120-4555-920B-B3931F1F079A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E271156-CE9D-42CA-90DB-67DE3603DB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="3870" windowWidth="23550" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="4620" windowWidth="23550" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week Counter" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Week 1</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Week 12</t>
   </si>
   <si>
-    <t>Week 1 Requirements</t>
-  </si>
-  <si>
     <t>Github Repository</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Use-Case Design</t>
   </si>
   <si>
-    <t>Week 2 Requirements</t>
-  </si>
-  <si>
     <t>Create Project</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
   </si>
   <si>
     <t>SQL Queries</t>
-  </si>
-  <si>
-    <t>Week 3 Requirements</t>
   </si>
   <si>
     <t>Connection Factory Utility</t>
@@ -486,7 +477,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -528,7 +519,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -563,9 +554,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -595,11 +588,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -612,42 +600,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -662,40 +645,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -720,32 +700,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>